<commit_message>
Addition of channel gate latest scripts
</commit_message>
<xml_diff>
--- a/testdata/CGFiles/ChannelGateTestData.xlsx
+++ b/testdata/CGFiles/ChannelGateTestData.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
+  <xr:revisionPtr documentId="13_ncr:1_{A1C5A59E-0ED2-4EC3-9AF1-AF1D2992592E}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="1" windowHeight="6330" windowWidth="13860" xWindow="0" yWindow="2520"/>
+    <workbookView activeTab="1" windowHeight="11160" windowWidth="20730" xWindow="-120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" r:id="rId1" sheetId="1"/>
@@ -16,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="149">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="173" uniqueCount="153">
   <si>
     <t>Useremail</t>
   </si>
@@ -66,9 +67,6 @@
     <t>UPC</t>
   </si>
   <si>
-    <t>US</t>
-  </si>
-  <si>
     <t>Wholesale</t>
   </si>
   <si>
@@ -294,15 +292,6 @@
     <t>036000291452</t>
   </si>
   <si>
-    <t>automation_sku_166</t>
-  </si>
-  <si>
-    <t>2266777</t>
-  </si>
-  <si>
-    <t>Test Automation Title 1629</t>
-  </si>
-  <si>
     <t>Aero</t>
   </si>
   <si>
@@ -402,77 +391,101 @@
     <t>5701234567899</t>
   </si>
   <si>
-    <t>Test Automation Title 19</t>
-  </si>
-  <si>
-    <t>automation_sku_60</t>
-  </si>
-  <si>
-    <t>2350956</t>
-  </si>
-  <si>
-    <t>Test Automation Title 85609</t>
-  </si>
-  <si>
-    <t>Test Automation Title 15</t>
-  </si>
-  <si>
-    <t>automation_sku_255</t>
-  </si>
-  <si>
-    <t>Test Automation Title 10</t>
-  </si>
-  <si>
-    <t>automation_sku_785</t>
-  </si>
-  <si>
-    <t>Test Automation Title 50127</t>
-  </si>
-  <si>
-    <t>2350957</t>
-  </si>
-  <si>
-    <t>automation_sku_204</t>
-  </si>
-  <si>
-    <t>Test Automation Title 32776</t>
-  </si>
-  <si>
-    <t>Test Automation Title 20</t>
-  </si>
-  <si>
-    <t>automation_sku_455</t>
-  </si>
-  <si>
-    <t>Test Automation Title 12</t>
-  </si>
-  <si>
-    <t>automation_sku_794</t>
-  </si>
-  <si>
-    <t>Test Automation Title 57935</t>
+    <t>United States</t>
+  </si>
+  <si>
+    <t>Content Score</t>
+  </si>
+  <si>
+    <t>47</t>
+  </si>
+  <si>
+    <t>2567402</t>
+  </si>
+  <si>
+    <t>29</t>
   </si>
   <si>
     <t>Test Automation Title 13</t>
   </si>
   <si>
-    <t>automation_sku_969</t>
-  </si>
-  <si>
-    <t>2389173</t>
-  </si>
-  <si>
-    <t>Test Automation Title 1209</t>
+    <t>automation_sku_777</t>
+  </si>
+  <si>
+    <t>Test Automation Title 279</t>
+  </si>
+  <si>
+    <t>automation_sku_250</t>
+  </si>
+  <si>
+    <t>Test Automation Title 520</t>
+  </si>
+  <si>
+    <t>automation_sku_582</t>
+  </si>
+  <si>
+    <t>Test Automation Title 26</t>
+  </si>
+  <si>
+    <t>automation_sku_112</t>
+  </si>
+  <si>
+    <t>Test Automation Title 636</t>
+  </si>
+  <si>
+    <t>automation_sku_363</t>
+  </si>
+  <si>
+    <t>2572945</t>
+  </si>
+  <si>
+    <t>Test Automation Title 690</t>
+  </si>
+  <si>
+    <t>automation_sku_560</t>
+  </si>
+  <si>
+    <t>Test Automation Title 862</t>
+  </si>
+  <si>
+    <t>automation_sku_626</t>
+  </si>
+  <si>
+    <t>2572946</t>
+  </si>
+  <si>
+    <t>Test Automation Title 89191</t>
+  </si>
+  <si>
+    <t>Test Automation Title 258</t>
+  </si>
+  <si>
+    <t>automation_sku_888</t>
+  </si>
+  <si>
+    <t>Test Automation Title 801</t>
+  </si>
+  <si>
+    <t>automation_sku_253</t>
+  </si>
+  <si>
+    <t>Test Automation Title 93</t>
+  </si>
+  <si>
+    <t>automation_sku_23</t>
+  </si>
+  <si>
+    <t>2577913</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -501,7 +514,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="58">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -518,11 +531,307 @@
         <fgColor indexed="9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="5">
+  <borders count="57">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -550,6 +859,196 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+    </border>
+    <border>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
+    <border>
       <top style="thin"/>
     </border>
     <border>
@@ -563,56 +1062,80 @@
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="43"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyProtection="0" borderId="0" fillId="0" fontId="3" numFmtId="164"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="43">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
     <xf applyAlignment="1" applyProtection="1" borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="2" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="2" fillId="3" fontId="0" numFmtId="0" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="3" fillId="4" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="4" fillId="5" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="2" quotePrefix="1" xfId="2">
+      <alignment vertical="top"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="top"/>
     </xf>
-    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="1" applyFill="1" borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" quotePrefix="1" xfId="2"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyBorder="true" applyFill="true" borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="true" applyBorder="true"/>
+    <xf applyBorder="1" applyFill="1" borderId="5" fillId="6" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFill="1" borderId="6" fillId="7" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="8" fillId="9" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="10" fillId="11" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="12" fillId="13" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="14" fillId="15" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="16" fillId="17" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="18" fillId="19" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="20" fillId="21" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="22" fillId="23" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="24" fillId="25" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="26" fillId="27" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="28" fillId="29" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="30" fillId="31" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="32" fillId="33" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="34" fillId="35" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="36" fillId="37" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="38" fillId="39" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="40" fillId="41" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="42" fillId="43" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="44" fillId="45" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="46" fillId="47" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="48" fillId="49" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="50" fillId="51" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="52" fillId="53" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="true" applyFill="true" borderId="54" fillId="55" fontId="0" numFmtId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="57" borderId="56" xfId="0" applyFill="true" applyBorder="true"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle builtinId="3" name="Comma" xfId="2"/>
@@ -621,6 +1144,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -667,7 +1198,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -699,9 +1230,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -733,6 +1282,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -908,21 +1475,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -933,7 +1500,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -944,63 +1511,79 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="A2"/>
-    <hyperlink r:id="rId2" ref="A3"/>
+    <hyperlink r:id="rId1" ref="A2" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink r:id="rId2" ref="A3" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
   </hyperlinks>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AS11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:AT11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B3" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="25.359375" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="10.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="6.140625" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="10.85546875" collapsed="true"/>
     <col min="5" max="5" bestFit="true" customWidth="true" width="35.5703125" collapsed="true"/>
     <col min="6" max="6" bestFit="true" customWidth="true" width="20.0625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="20.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
     <col min="8" max="8" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" style="2" width="61.5703125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="7.28515625" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="7.0" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="5.5703125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="6.0" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="8.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="8.0" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" style="2" width="108.28515625" collapsed="true"/>
     <col min="17" max="17" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="30.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="25.85546875" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="69.140625" collapsed="true"/>
     <col min="20" max="20" bestFit="true" customWidth="true" width="23.28515625" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="21.140625" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
-    <col min="24" max="24" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="7.140625" collapsed="true"/>
     <col min="26" max="26" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
     <col min="27" max="27" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
     <col min="28" max="28" bestFit="true" customWidth="true" width="14.0" collapsed="true"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="14.28515625" collapsed="true"/>
     <col min="30" max="30" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="6.85546875" collapsed="true"/>
+    <col min="32" max="33" bestFit="true" customWidth="true" width="6.42578125" collapsed="true"/>
+    <col min="34" max="34" bestFit="true" customWidth="true" width="7.42578125" collapsed="true"/>
+    <col min="35" max="35" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="36" max="37" bestFit="true" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="4.5703125" collapsed="true"/>
     <col min="40" max="40" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
     <col min="41" max="41" bestFit="true" customWidth="true" width="12.0" collapsed="true"/>
     <col min="42" max="44" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
+    <col min="45" max="45" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:44">
+    <row r="1" spans="1:45" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>8</v>
@@ -1018,123 +1601,126 @@
         <v>15</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K1" s="4" t="s">
+      <c r="M1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="P1" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="Q1" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="R1" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="Z1" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="T1" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="U1" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="Y1" s="3" t="s">
+      <c r="AA1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="AC1" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="AD1" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="AE1" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="AF1" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="AI1" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="Z1" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="AD1" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="AE1" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="AF1" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="AG1" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AJ1" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AM1" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="AI1" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="AJ1" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="AK1" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AL1" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="AN1" s="3" t="s">
+      <c r="AO1" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="AO1" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="AP1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="AQ1" s="3" t="s">
+      <c r="AR1" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="AR1" t="s">
-        <v>88</v>
+      <c r="AS1" s="7" t="s">
+        <v>125</v>
       </c>
     </row>
-    <row ht="90" r="2" spans="1:44">
-      <c r="A2" s="35" t="s">
-        <v>148</v>
-      </c>
-      <c r="B2" s="36" t="s">
-        <v>147</v>
+    <row ht="60" r="2" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" s="41" t="s">
+        <v>152</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>11</v>
@@ -1145,297 +1731,655 @@
       <c r="E2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="F2" s="33" t="s">
-        <v>146</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>85</v>
+      <c r="F2" s="40" t="s">
+        <v>151</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>84</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J2" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="K2" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="M2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="M2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="T2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="U2" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z2" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AB2" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="AC2" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="AD2" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="AE2" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="AF2" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH2" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="AI2" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="AJ2" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="AK2" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="AL2" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="AM2" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="AN2" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AP2" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ2" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="AR2" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="AS2" s="42" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row ht="120" r="3" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A3" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="F3" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="M3" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="O3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="S2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="T2" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="U2" s="6" t="s">
+      <c r="P3" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="S3" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="U3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="V3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="W3" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="V2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="W2" s="3" t="s">
+      <c r="X3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z3" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="AA3" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="Y2" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z2" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="AA2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="AC2" s="6" t="s">
+      <c r="AB3" s="9">
+        <v>1</v>
+      </c>
+      <c r="AC3" s="9">
+        <v>2</v>
+      </c>
+      <c r="AD3" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="AD2" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE2" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="AF2" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="AG2" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ2" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="AK2" s="6" t="s">
-        <v>69</v>
-      </c>
-      <c r="AL2" s="6" t="s">
+      <c r="AE3" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="AF3" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="AG3" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="AH3" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="AI3" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="AJ3" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="AK3" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="AL3" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="AM3" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="AM2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO2" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="AP2" s="6" t="s">
+      <c r="AN3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="AO3" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="AP3" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="AQ3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="AQ2" s="6" t="s">
+      <c r="AR3" s="9" t="s">
         <v>90</v>
       </c>
-      <c r="AR2" s="6" t="s">
-        <v>91</v>
+      <c r="AS3" s="12" t="s">
+        <v>126</v>
       </c>
     </row>
-    <row ht="225" r="3" spans="1:44">
-      <c r="A3" s="11" t="s">
+    <row r="4" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A4" s="6"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="13" t="s">
+        <v>116</v>
+      </c>
+      <c r="H4" s="6"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+      <c r="N4" s="6"/>
+      <c r="O4" s="6"/>
+      <c r="P4" s="14"/>
+      <c r="Q4" s="6"/>
+      <c r="R4" s="6"/>
+      <c r="S4" s="6"/>
+      <c r="T4" s="6"/>
+      <c r="U4" s="6"/>
+      <c r="V4" s="6"/>
+      <c r="W4" s="6"/>
+      <c r="X4" s="6"/>
+      <c r="Y4" s="6"/>
+      <c r="Z4" s="6"/>
+      <c r="AA4" s="6"/>
+      <c r="AB4" s="6"/>
+      <c r="AC4" s="6"/>
+      <c r="AD4" s="6"/>
+      <c r="AE4" s="6"/>
+      <c r="AF4" s="6"/>
+      <c r="AG4" s="6"/>
+      <c r="AH4" s="6"/>
+      <c r="AI4" s="6"/>
+      <c r="AJ4" s="6"/>
+      <c r="AK4" s="6"/>
+      <c r="AL4" s="6"/>
+      <c r="AM4" s="6"/>
+      <c r="AN4" s="6"/>
+      <c r="AO4" s="6"/>
+      <c r="AP4" s="6"/>
+      <c r="AQ4" s="6"/>
+      <c r="AR4" s="6"/>
+      <c r="AS4" s="15"/>
+    </row>
+    <row r="5" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="6"/>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="13" t="s">
+        <v>117</v>
+      </c>
+      <c r="H5" s="6"/>
+      <c r="I5" s="6"/>
+      <c r="J5" s="6"/>
+      <c r="K5" s="6"/>
+      <c r="L5" s="6"/>
+      <c r="M5" s="6"/>
+      <c r="N5" s="6"/>
+      <c r="O5" s="6"/>
+      <c r="P5" s="14"/>
+      <c r="Q5" s="6"/>
+      <c r="R5" s="6"/>
+      <c r="S5" s="6"/>
+      <c r="T5" s="6"/>
+      <c r="U5" s="6"/>
+      <c r="V5" s="6"/>
+      <c r="W5" s="6"/>
+      <c r="X5" s="6"/>
+      <c r="Y5" s="6"/>
+      <c r="Z5" s="6"/>
+      <c r="AA5" s="6"/>
+      <c r="AB5" s="6"/>
+      <c r="AC5" s="6"/>
+      <c r="AD5" s="6"/>
+      <c r="AE5" s="6"/>
+      <c r="AF5" s="6"/>
+      <c r="AG5" s="6"/>
+      <c r="AH5" s="6"/>
+      <c r="AI5" s="6"/>
+      <c r="AJ5" s="6"/>
+      <c r="AK5" s="6"/>
+      <c r="AL5" s="6"/>
+      <c r="AM5" s="6"/>
+      <c r="AN5" s="6"/>
+      <c r="AO5" s="6"/>
+      <c r="AP5" s="6"/>
+      <c r="AQ5" s="6"/>
+      <c r="AR5" s="6"/>
+      <c r="AS5" s="15"/>
+    </row>
+    <row r="6" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A6" s="6"/>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="13" t="s">
+        <v>118</v>
+      </c>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+      <c r="K6" s="6"/>
+      <c r="L6" s="6"/>
+      <c r="M6" s="6"/>
+      <c r="N6" s="6"/>
+      <c r="O6" s="6"/>
+      <c r="P6" s="14"/>
+      <c r="Q6" s="6"/>
+      <c r="R6" s="6"/>
+      <c r="S6" s="6"/>
+      <c r="T6" s="6"/>
+      <c r="U6" s="6"/>
+      <c r="V6" s="6"/>
+      <c r="W6" s="6"/>
+      <c r="X6" s="6"/>
+      <c r="Y6" s="6"/>
+      <c r="Z6" s="6"/>
+      <c r="AA6" s="6"/>
+      <c r="AB6" s="6"/>
+      <c r="AC6" s="6"/>
+      <c r="AD6" s="6"/>
+      <c r="AE6" s="6"/>
+      <c r="AF6" s="6"/>
+      <c r="AG6" s="6"/>
+      <c r="AH6" s="6"/>
+      <c r="AI6" s="6"/>
+      <c r="AJ6" s="6"/>
+      <c r="AK6" s="6"/>
+      <c r="AL6" s="6"/>
+      <c r="AM6" s="6"/>
+      <c r="AN6" s="6"/>
+      <c r="AO6" s="6"/>
+      <c r="AP6" s="6"/>
+      <c r="AQ6" s="6"/>
+      <c r="AR6" s="6"/>
+      <c r="AS6" s="15"/>
+    </row>
+    <row r="7" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A7" s="6"/>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
+      <c r="G7" s="13" t="s">
         <v>119</v>
       </c>
-      <c r="B3" s="12" t="s">
-        <v>118</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>117</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="J3" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="K3" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="L3" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="M3" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="N3" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="P3" s="5" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="R3" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="S3" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="T3" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="U3" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="V3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="W3" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="X3" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="Y3" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="Z3" s="6" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA3" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AB3" s="6">
-        <v>1</v>
-      </c>
-      <c r="AC3" s="6">
-        <v>2</v>
-      </c>
-      <c r="AD3" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="AE3" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="AF3" s="6" t="s">
-        <v>105</v>
-      </c>
-      <c r="AG3" s="6" t="s">
-        <v>106</v>
-      </c>
-      <c r="AH3" s="6" t="s">
-        <v>107</v>
-      </c>
-      <c r="AI3" s="6" t="s">
-        <v>110</v>
-      </c>
-      <c r="AJ3" s="6" t="s">
-        <v>108</v>
-      </c>
-      <c r="AK3" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="AL3" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM3" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="AN3" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="AO3" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="AP3" s="6" t="s">
-        <v>89</v>
-      </c>
-      <c r="AQ3" s="6" t="s">
-        <v>90</v>
-      </c>
-      <c r="AR3" s="6" t="s">
-        <v>91</v>
-      </c>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
+      <c r="M7" s="6"/>
+      <c r="N7" s="6"/>
+      <c r="O7" s="6"/>
+      <c r="P7" s="14"/>
+      <c r="Q7" s="6"/>
+      <c r="R7" s="6"/>
+      <c r="S7" s="6"/>
+      <c r="T7" s="6"/>
+      <c r="U7" s="6"/>
+      <c r="V7" s="6"/>
+      <c r="W7" s="6"/>
+      <c r="X7" s="6"/>
+      <c r="Y7" s="6"/>
+      <c r="Z7" s="6"/>
+      <c r="AA7" s="6"/>
+      <c r="AB7" s="6"/>
+      <c r="AC7" s="6"/>
+      <c r="AD7" s="6"/>
+      <c r="AE7" s="6"/>
+      <c r="AF7" s="6"/>
+      <c r="AG7" s="6"/>
+      <c r="AH7" s="6"/>
+      <c r="AI7" s="6"/>
+      <c r="AJ7" s="6"/>
+      <c r="AK7" s="6"/>
+      <c r="AL7" s="6"/>
+      <c r="AM7" s="6"/>
+      <c r="AN7" s="6"/>
+      <c r="AO7" s="6"/>
+      <c r="AP7" s="6"/>
+      <c r="AQ7" s="6"/>
+      <c r="AR7" s="6"/>
+      <c r="AS7" s="15"/>
     </row>
-    <row r="4" spans="1:44">
-      <c r="G4" s="13" t="s">
+    <row r="8" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A8" s="6"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="13" t="s">
         <v>120</v>
       </c>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
+      <c r="L8" s="6"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
+      <c r="O8" s="6"/>
+      <c r="P8" s="14"/>
+      <c r="Q8" s="6"/>
+      <c r="R8" s="6"/>
+      <c r="S8" s="6"/>
+      <c r="T8" s="6"/>
+      <c r="U8" s="6"/>
+      <c r="V8" s="6"/>
+      <c r="W8" s="6"/>
+      <c r="X8" s="6"/>
+      <c r="Y8" s="6"/>
+      <c r="Z8" s="6"/>
+      <c r="AA8" s="6"/>
+      <c r="AB8" s="6"/>
+      <c r="AC8" s="6"/>
+      <c r="AD8" s="6"/>
+      <c r="AE8" s="6"/>
+      <c r="AF8" s="6"/>
+      <c r="AG8" s="6"/>
+      <c r="AH8" s="6"/>
+      <c r="AI8" s="6"/>
+      <c r="AJ8" s="6"/>
+      <c r="AK8" s="6"/>
+      <c r="AL8" s="6"/>
+      <c r="AM8" s="6"/>
+      <c r="AN8" s="6"/>
+      <c r="AO8" s="6"/>
+      <c r="AP8" s="6"/>
+      <c r="AQ8" s="6"/>
+      <c r="AR8" s="6"/>
+      <c r="AS8" s="15"/>
     </row>
-    <row r="5" spans="1:44">
-      <c r="G5" s="13" t="s">
+    <row r="9" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A9" s="6"/>
+      <c r="B9" s="6"/>
+      <c r="C9" s="6"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
+      <c r="G9" s="13" t="s">
         <v>121</v>
       </c>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="14"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="15"/>
     </row>
-    <row r="6" spans="1:44">
-      <c r="G6" s="13" t="s">
+    <row r="10" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A10" s="6"/>
+      <c r="B10" s="6"/>
+      <c r="C10" s="6"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="13" t="s">
         <v>122</v>
       </c>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
+      <c r="K10" s="6"/>
+      <c r="L10" s="6"/>
+      <c r="M10" s="6"/>
+      <c r="N10" s="6"/>
+      <c r="O10" s="6"/>
+      <c r="P10" s="14"/>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
+      <c r="S10" s="6"/>
+      <c r="T10" s="6"/>
+      <c r="U10" s="6"/>
+      <c r="V10" s="6"/>
+      <c r="W10" s="6"/>
+      <c r="X10" s="6"/>
+      <c r="Y10" s="6"/>
+      <c r="Z10" s="6"/>
+      <c r="AA10" s="6"/>
+      <c r="AB10" s="6"/>
+      <c r="AC10" s="6"/>
+      <c r="AD10" s="6"/>
+      <c r="AE10" s="6"/>
+      <c r="AF10" s="6"/>
+      <c r="AG10" s="6"/>
+      <c r="AH10" s="6"/>
+      <c r="AI10" s="6"/>
+      <c r="AJ10" s="6"/>
+      <c r="AK10" s="6"/>
+      <c r="AL10" s="6"/>
+      <c r="AM10" s="6"/>
+      <c r="AN10" s="6"/>
+      <c r="AO10" s="6"/>
+      <c r="AP10" s="6"/>
+      <c r="AQ10" s="6"/>
+      <c r="AR10" s="6"/>
+      <c r="AS10" s="15"/>
     </row>
-    <row r="7" spans="1:44">
-      <c r="G7" s="13" t="s">
+    <row r="11" spans="1:45" x14ac:dyDescent="0.25">
+      <c r="A11" s="6"/>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
+      <c r="G11" s="13" t="s">
         <v>123</v>
       </c>
-    </row>
-    <row r="8" spans="1:44">
-      <c r="G8" s="13" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="9" spans="1:44">
-      <c r="G9" s="13" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="10" spans="1:44">
-      <c r="G10" s="13" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="11" spans="1:44">
-      <c r="G11" s="13" t="s">
-        <v>127</v>
-      </c>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
+      <c r="K11" s="6"/>
+      <c r="L11" s="6"/>
+      <c r="M11" s="6"/>
+      <c r="N11" s="6"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="14"/>
+      <c r="Q11" s="6"/>
+      <c r="R11" s="6"/>
+      <c r="S11" s="6"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
+      <c r="V11" s="6"/>
+      <c r="W11" s="6"/>
+      <c r="X11" s="6"/>
+      <c r="Y11" s="6"/>
+      <c r="Z11" s="6"/>
+      <c r="AA11" s="6"/>
+      <c r="AB11" s="6"/>
+      <c r="AC11" s="6"/>
+      <c r="AD11" s="6"/>
+      <c r="AE11" s="6"/>
+      <c r="AF11" s="6"/>
+      <c r="AG11" s="6"/>
+      <c r="AH11" s="6"/>
+      <c r="AI11" s="6"/>
+      <c r="AJ11" s="6"/>
+      <c r="AK11" s="6"/>
+      <c r="AL11" s="6"/>
+      <c r="AM11" s="6"/>
+      <c r="AN11" s="6"/>
+      <c r="AO11" s="6"/>
+      <c r="AP11" s="6"/>
+      <c r="AQ11" s="6"/>
+      <c r="AR11" s="6"/>
+      <c r="AS11" s="15"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
@@ -1444,12 +2388,12 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>